<commit_message>
Buscando no Scopus, excelentes resultados
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Plácido\Documents\Faculdade\11 Semestre\Gestao de Qualidade\Artigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECA411E-29CA-44A6-AAFD-D01C04F4D19A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560CF1E7-2CB1-4993-B535-908FFD49DDE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Metodologia" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>Uso de Redes Neurais no Contexto da Sustentabilidade</t>
   </si>
@@ -114,24 +115,12 @@
     <t>Neural Network Sustainable Developing</t>
   </si>
   <si>
-    <t>Neural Network Environmental Sustaintability</t>
-  </si>
-  <si>
     <t>Springer</t>
   </si>
   <si>
-    <t>"Neural Network" AND "Sustentability"</t>
-  </si>
-  <si>
-    <t>"Neural Network" AND "Sustainable Developing"</t>
-  </si>
-  <si>
     <t>"Neural Network" AND "Environment"</t>
   </si>
   <si>
-    <t>"Neural Network" AND "Environmental Sustaintability"</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -151,6 +140,24 @@
   </si>
   <si>
     <t>Review Articles, Research Articles or Case Reports</t>
+  </si>
+  <si>
+    <t>Neural Network Environmental Sustainability</t>
+  </si>
+  <si>
+    <t>Review, Research and Case reports</t>
+  </si>
+  <si>
+    <t>Número de Artigos Analisados</t>
+  </si>
+  <si>
+    <t>"Neural Network" AND "Sustainability"</t>
+  </si>
+  <si>
+    <t>"Neural Network" AND "Sustainable Development"</t>
+  </si>
+  <si>
+    <t>"Neural Network" AND "Environmental Sustainability"</t>
   </si>
 </sst>
 </file>
@@ -220,10 +227,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="24"/>
-      <color rgb="FF505050"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="8">
@@ -270,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -287,11 +294,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -301,6 +321,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -313,26 +339,458 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -486,70 +944,90 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E9082B0C-C77E-4144-ABB3-2AFCBC27B540}" name="Table3" displayName="Table3" ref="E2:K10" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="E2:K10" xr:uid="{B010B902-4089-4EDF-95EA-6510DE3263AD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E9082B0C-C77E-4144-ABB3-2AFCBC27B540}" name="Table3" displayName="Table3" ref="E2:K11" totalsRowShown="0" headerRowDxfId="36">
+  <autoFilter ref="E2:K11" xr:uid="{B010B902-4089-4EDF-95EA-6510DE3263AD}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{150631A9-22E1-47B0-BF0B-E3226545937F}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{8DCACCD9-6A27-420A-A5EC-D230FB3DD3E1}" name="Science Direct"/>
-    <tableColumn id="3" xr3:uid="{6641DD30-BFF3-4387-9774-4A7558C8F975}" name="Emerald Insight"/>
-    <tableColumn id="4" xr3:uid="{DAD195B6-9347-4529-B450-D73CCDFBE75D}" name="Scopus"/>
-    <tableColumn id="5" xr3:uid="{34F20F22-9351-4481-935A-8C2745791DD0}" name="Springler"/>
-    <tableColumn id="6" xr3:uid="{BB081D5A-5346-4547-A641-31761151FB9D}" name="Wiley"/>
-    <tableColumn id="7" xr3:uid="{4636F687-F30B-485D-8A92-E748AD5C8912}" name="Taylor &amp; Francis"/>
+    <tableColumn id="1" xr3:uid="{150631A9-22E1-47B0-BF0B-E3226545937F}" name="Column1">
+      <calculatedColumnFormula>C2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{8DCACCD9-6A27-420A-A5EC-D230FB3DD3E1}" name="Science Direct" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{6641DD30-BFF3-4387-9774-4A7558C8F975}" name="Emerald Insight" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{DAD195B6-9347-4529-B450-D73CCDFBE75D}" name="Scopus" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{34F20F22-9351-4481-935A-8C2745791DD0}" name="Springler" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{BB081D5A-5346-4547-A641-31761151FB9D}" name="Wiley" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{4636F687-F30B-485D-8A92-E748AD5C8912}" name="Taylor &amp; Francis" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6F8EB86C-85F1-4FBA-9FFC-B6D0058B3592}" name="Table35" displayName="Table35" ref="E13:K21" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6F8EB86C-85F1-4FBA-9FFC-B6D0058B3592}" name="Table35" displayName="Table35" ref="E13:K21" totalsRowShown="0" headerRowDxfId="35">
   <autoFilter ref="E13:K21" xr:uid="{6D5004CA-553C-49B0-B5A0-226275053A1F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B76494C4-2327-4899-8567-C3C05E8F4CC7}" name="Column1">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D309A7D0-64F5-49E2-82A9-6BC2F06609A7}" name="Science Direct"/>
-    <tableColumn id="3" xr3:uid="{8BB7FCBA-BACA-4910-9EF8-AB91065EFC17}" name="Emerald Insight"/>
-    <tableColumn id="4" xr3:uid="{F918F495-5DA6-40C8-A18D-8D0ACDA320FD}" name="Scopus"/>
-    <tableColumn id="5" xr3:uid="{5D0BBA33-8122-4273-9318-6B04EBDE10E2}" name="Springler"/>
-    <tableColumn id="6" xr3:uid="{3B6A5EB3-0DE5-4170-9759-9BF25C23241A}" name="Wiley"/>
-    <tableColumn id="7" xr3:uid="{170F1506-26AC-4697-8E2E-935DBA2D536D}" name="Taylor &amp; Francis"/>
+    <tableColumn id="2" xr3:uid="{D309A7D0-64F5-49E2-82A9-6BC2F06609A7}" name="Science Direct" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{8BB7FCBA-BACA-4910-9EF8-AB91065EFC17}" name="Emerald Insight" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{F918F495-5DA6-40C8-A18D-8D0ACDA320FD}" name="Scopus" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{5D0BBA33-8122-4273-9318-6B04EBDE10E2}" name="Springler" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{3B6A5EB3-0DE5-4170-9759-9BF25C23241A}" name="Wiley" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{170F1506-26AC-4697-8E2E-935DBA2D536D}" name="Taylor &amp; Francis" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CD1481DA-7A29-4C6A-99A4-BB9A73AC5AAE}" name="Table356" displayName="Table356" ref="E24:K32" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CD1481DA-7A29-4C6A-99A4-BB9A73AC5AAE}" name="Table356" displayName="Table356" ref="E24:K32" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="E24:K32" xr:uid="{325C82D0-9CFB-45D4-A270-FC6432082374}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{24654240-E379-4C9A-9DCD-65C789D335AB}" name="Column1">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{639EB9D1-B2B4-4E0F-8725-AFB812C9A65D}" name="Science Direct"/>
-    <tableColumn id="3" xr3:uid="{BDA00B13-6195-44C0-99E4-22674588FB32}" name="Emerald Insight"/>
-    <tableColumn id="4" xr3:uid="{CD7A3BC0-4322-4169-B82B-92D2BCD379A0}" name="Scopus"/>
-    <tableColumn id="5" xr3:uid="{AEB54831-9168-44FC-A3FB-36C3901C1772}" name="Springler"/>
-    <tableColumn id="6" xr3:uid="{9D108FDF-29DF-4855-825C-22556E2C6F9F}" name="Wiley"/>
-    <tableColumn id="7" xr3:uid="{DC271623-6492-4738-A374-609DED940358}" name="Taylor &amp; Francis"/>
+    <tableColumn id="2" xr3:uid="{639EB9D1-B2B4-4E0F-8725-AFB812C9A65D}" name="Science Direct" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{BDA00B13-6195-44C0-99E4-22674588FB32}" name="Emerald Insight" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{CD7A3BC0-4322-4169-B82B-92D2BCD379A0}" name="Scopus" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{AEB54831-9168-44FC-A3FB-36C3901C1772}" name="Springler" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{9D108FDF-29DF-4855-825C-22556E2C6F9F}" name="Wiley" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{DC271623-6492-4738-A374-609DED940358}" name="Taylor &amp; Francis" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AC928D1D-B98E-40EA-A207-C233D64396A2}" name="Table37" displayName="Table37" ref="M34:S42" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AC928D1D-B98E-40EA-A207-C233D64396A2}" name="Table37" displayName="Table37" ref="M34:S42" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="M34:S42" xr:uid="{67ACFE52-40D3-4D5B-9587-380B01CA9349}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CC58C69A-3BD4-439F-8E2A-78CFCFA772E9}" name="Column1" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{CC58C69A-3BD4-439F-8E2A-78CFCFA772E9}" name="Column1" dataDxfId="31">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{6752AC08-A118-44B2-9200-921CA1F8335B}" name="Science Direct" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{0472B21D-97B3-421D-B264-C2DE2E81F3BF}" name="Emerald Insight" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{EDB81E1A-540C-49BE-8621-D2F785CFDE5E}" name="Scopus" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{F477D8B8-98A5-4C44-83F3-C0FFBA22D4AD}" name="Springler" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{F947E302-3405-4752-8179-B2C47811F385}" name="Wiley" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{08B07A72-C239-4B61-91DE-CF31F091EA4B}" name="Taylor &amp; Francis" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{6752AC08-A118-44B2-9200-921CA1F8335B}" name="Science Direct" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{0472B21D-97B3-421D-B264-C2DE2E81F3BF}" name="Emerald Insight" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{EDB81E1A-540C-49BE-8621-D2F785CFDE5E}" name="Scopus" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{F477D8B8-98A5-4C44-83F3-C0FFBA22D4AD}" name="Springler" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{F947E302-3405-4752-8179-B2C47811F385}" name="Wiley" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{08B07A72-C239-4B61-91DE-CF31F091EA4B}" name="Taylor &amp; Francis" dataDxfId="25"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{49435503-B1E7-4724-AFF1-275C704DC8E8}" name="Table33" displayName="Table33" ref="M13:S21" totalsRowShown="0" headerRowDxfId="24">
+  <autoFilter ref="M13:S21" xr:uid="{1928454F-FA0E-4F92-AA13-866388A59E12}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{D56F5F81-C1E6-46F7-ADE0-F94365FD3D3D}" name="Column1">
+      <calculatedColumnFormula>C2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{611CC9E7-DBC7-4A7A-AED8-479F52685EA4}" name="Science Direct" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{EEDB19DA-96B1-4BE3-A9E8-30B7950DCCA0}" name="Emerald Insight" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{232281CB-02F4-4E71-8764-3B40A5B0AA63}" name="Scopus" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{3686983C-0E8E-47E0-974B-7884E8A32FE1}" name="Springler" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{B64EF221-003C-4B41-9901-A7FC32144AE1}" name="Wiley" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{CA984F23-3162-4D75-BE65-53769D2B4FF8}" name="Taylor &amp; Francis" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -855,7 +1333,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,14 +1360,14 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="9" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="10"/>
+      <c r="M1" s="12"/>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -903,10 +1381,10 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="12"/>
+      <c r="K2" s="14"/>
       <c r="L2" s="6" t="s">
         <v>7</v>
       </c>
@@ -915,10 +1393,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="12"/>
+      <c r="K3" s="14"/>
       <c r="L3" s="6" t="s">
         <v>8</v>
       </c>
@@ -927,10 +1405,10 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="12"/>
+      <c r="K4" s="14"/>
       <c r="L4" s="6" t="s">
         <v>9</v>
       </c>
@@ -978,24 +1456,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="51" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="42.42578125" customWidth="1"/>
+    <col min="13" max="13" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -1003,7 +1481,7 @@
     <col min="19" max="19" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -1011,46 +1489,46 @@
         <v>15</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+        <v>30</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
       <c r="L1" s="8"/>
     </row>
-    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -1061,11 +1539,20 @@
         <f>C2</f>
         <v>Neural Network Sustainability</v>
       </c>
-      <c r="F3" s="16">
-        <v>55.387</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F3" s="18">
+        <v>55623</v>
+      </c>
+      <c r="G3" s="19">
+        <v>627</v>
+      </c>
+      <c r="H3" s="19">
+        <v>497</v>
+      </c>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -1073,379 +1560,692 @@
         <v>25</v>
       </c>
       <c r="E4" t="str">
-        <f>C3</f>
+        <f t="shared" ref="E4:E10" si="0">C3</f>
         <v>Neural Network Sustainable Developing</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F4" s="19">
+        <v>44376</v>
+      </c>
+      <c r="G4" s="19">
+        <v>1052</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
         <v>27</v>
       </c>
+      <c r="C5" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="E5" t="str">
-        <f>C4</f>
+        <f t="shared" si="0"/>
         <v>Neural Network Environment</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F5" s="19"/>
+      <c r="G5" s="19">
+        <v>3278</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E6" t="str">
-        <f>C5</f>
-        <v>Neural Network Environmental Sustaintability</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>Neural Network Environmental Sustainability</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>"Neural Network" AND "Sustainability"</v>
+      </c>
+      <c r="F7" s="18">
+        <v>17490</v>
+      </c>
+      <c r="G7" s="19">
+        <v>123</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>"Neural Network" AND "Sustainable Development"</v>
+      </c>
+      <c r="F8" s="19">
+        <v>2557</v>
+      </c>
+      <c r="G8" s="19">
+        <v>66</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>"Neural Network" AND "Environment"</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>"Neural Network" AND "Environmental Sustainability"</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f>C10</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+      <c r="E12" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="M12" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="16">
-        <v>27.344000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="E12" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E14" t="str">
         <f>C2</f>
         <v>Neural Network Sustainability</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="18">
+        <v>27983</v>
+      </c>
+      <c r="G14" s="19">
+        <v>627</v>
+      </c>
+      <c r="H14" s="19">
+        <v>260</v>
+      </c>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="M14" t="str">
+        <f>C2</f>
+        <v>Neural Network Sustainability</v>
+      </c>
+      <c r="N14" s="18">
+        <v>125</v>
+      </c>
+      <c r="O14" s="19">
+        <v>60</v>
+      </c>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E15" t="str">
-        <f t="shared" ref="E15:E21" si="0">C3</f>
+        <f t="shared" ref="E15:E21" si="1">C3</f>
         <v>Neural Network Sustainable Developing</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F15" s="19">
+        <v>22709</v>
+      </c>
+      <c r="G15" s="19">
+        <v>1052</v>
+      </c>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="M15" t="str">
+        <f t="shared" ref="M15:M21" si="2">C3</f>
+        <v>Neural Network Sustainable Developing</v>
+      </c>
+      <c r="N15" s="19">
+        <v>75</v>
+      </c>
+      <c r="O15" s="19">
+        <v>100</v>
+      </c>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Neural Network Environment</v>
       </c>
-    </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F16" s="19"/>
+      <c r="G16" s="19">
+        <v>3278</v>
+      </c>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="M16" t="str">
+        <f t="shared" si="2"/>
+        <v>Neural Network Environment</v>
+      </c>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19">
+        <v>65</v>
+      </c>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+    </row>
+    <row r="17" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v>Neural Network Environmental Sustaintability</v>
-      </c>
-    </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>Neural Network Environmental Sustainability</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="M17" t="str">
+        <f t="shared" si="2"/>
+        <v>Neural Network Environmental Sustainability</v>
+      </c>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+    </row>
+    <row r="18" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>"Neural Network" AND "Sustentability"</v>
-      </c>
-    </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>"Neural Network" AND "Sustainability"</v>
+      </c>
+      <c r="F18" s="18">
+        <v>15635</v>
+      </c>
+      <c r="G18" s="19">
+        <v>123</v>
+      </c>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="M18" t="str">
+        <f t="shared" si="2"/>
+        <v>"Neural Network" AND "Sustainability"</v>
+      </c>
+      <c r="N18" s="18">
+        <v>150</v>
+      </c>
+      <c r="O18" s="19">
+        <v>50</v>
+      </c>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+    </row>
+    <row r="19" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v>"Neural Network" AND "Sustainable Developing"</v>
-      </c>
-    </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>"Neural Network" AND "Sustainable Development"</v>
+      </c>
+      <c r="F19" s="19">
+        <v>1741</v>
+      </c>
+      <c r="G19" s="19">
+        <v>66</v>
+      </c>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="M19" t="str">
+        <f t="shared" si="2"/>
+        <v>"Neural Network" AND "Sustainable Development"</v>
+      </c>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+    </row>
+    <row r="20" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>"Neural Network" AND "Environment"</v>
       </c>
-    </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="M20" t="str">
+        <f t="shared" si="2"/>
+        <v>"Neural Network" AND "Environment"</v>
+      </c>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+    </row>
+    <row r="21" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E21" t="str">
-        <f t="shared" si="0"/>
-        <v>"Neural Network" AND "Environmental Sustaintability"</v>
-      </c>
-    </row>
-    <row r="23" spans="5:11" ht="21" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>"Neural Network" AND "Environmental Sustainability"</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="M21" t="str">
+        <f t="shared" si="2"/>
+        <v>"Neural Network" AND "Environmental Sustainability"</v>
+      </c>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+    </row>
+    <row r="23" spans="5:19" ht="21" x14ac:dyDescent="0.35">
       <c r="E23" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-    </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+    </row>
+    <row r="24" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E25" t="str">
         <f>C2</f>
         <v>Neural Network Sustainability</v>
       </c>
-    </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F25" s="18"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+    </row>
+    <row r="26" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E26" t="str">
-        <f t="shared" ref="E26:E32" si="1">C3</f>
+        <f t="shared" ref="E26:E32" si="3">C3</f>
         <v>Neural Network Sustainable Developing</v>
       </c>
-    </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+    </row>
+    <row r="27" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Neural Network Environment</v>
       </c>
-    </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+    </row>
+    <row r="28" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
-        <v>Neural Network Environmental Sustaintability</v>
-      </c>
-    </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>Neural Network Environmental Sustainability</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+    </row>
+    <row r="29" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
-        <v>"Neural Network" AND "Sustentability"</v>
-      </c>
-    </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>"Neural Network" AND "Sustainability"</v>
+      </c>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+    </row>
+    <row r="30" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
-        <v>"Neural Network" AND "Sustainable Developing"</v>
-      </c>
-    </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>"Neural Network" AND "Sustainable Development"</v>
+      </c>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+    </row>
+    <row r="31" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"Neural Network" AND "Environment"</v>
       </c>
-    </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+    </row>
+    <row r="32" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
-        <v>"Neural Network" AND "Environmental Sustaintability"</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>"Neural Network" AND "Environmental Sustainability"</v>
+      </c>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
     </row>
     <row r="33" spans="13:19" ht="21" x14ac:dyDescent="0.35">
       <c r="M33" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
     </row>
     <row r="34" spans="13:19" x14ac:dyDescent="0.25">
       <c r="M34" t="s">
-        <v>33</v>
-      </c>
-      <c r="N34" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="N34" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="O34" s="13" t="s">
+      <c r="O34" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="P34" s="13" t="s">
+      <c r="P34" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Q34" s="13" t="s">
+      <c r="Q34" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R34" s="13" t="s">
+      <c r="R34" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="S34" s="13" t="s">
+      <c r="S34" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="13:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="M35" s="17" t="str">
-        <f>C2</f>
+    <row r="35" spans="13:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="M35" s="10" t="str">
+        <f t="shared" ref="M35:M42" si="4">C2</f>
         <v>Neural Network Sustainability</v>
       </c>
-      <c r="N35" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="O35" s="17"/>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
-      <c r="R35" s="17"/>
-      <c r="S35" s="17"/>
+      <c r="N35" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
     </row>
     <row r="36" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M36" s="17" t="str">
-        <f>C3</f>
+      <c r="M36" s="10" t="str">
+        <f t="shared" si="4"/>
         <v>Neural Network Sustainable Developing</v>
       </c>
-      <c r="N36" s="17"/>
-      <c r="O36" s="17"/>
-      <c r="P36" s="17"/>
-      <c r="Q36" s="17"/>
-      <c r="R36" s="17"/>
-      <c r="S36" s="17"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
     </row>
     <row r="37" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M37" s="17" t="str">
-        <f>C4</f>
+      <c r="M37" s="10" t="str">
+        <f t="shared" si="4"/>
         <v>Neural Network Environment</v>
       </c>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="17"/>
-      <c r="R37" s="17"/>
-      <c r="S37" s="17"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
     </row>
     <row r="38" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M38" s="17" t="str">
-        <f>C5</f>
-        <v>Neural Network Environmental Sustaintability</v>
-      </c>
-      <c r="N38" s="17"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
-      <c r="Q38" s="17"/>
-      <c r="R38" s="17"/>
-      <c r="S38" s="17"/>
+      <c r="M38" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>Neural Network Environmental Sustainability</v>
+      </c>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
     </row>
     <row r="39" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M39" s="17" t="str">
-        <f>C6</f>
-        <v>"Neural Network" AND "Sustentability"</v>
-      </c>
-      <c r="N39" s="17"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17"/>
-      <c r="Q39" s="17"/>
-      <c r="R39" s="17"/>
-      <c r="S39" s="17"/>
+      <c r="M39" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>"Neural Network" AND "Sustainability"</v>
+      </c>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
     </row>
     <row r="40" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M40" s="17" t="str">
-        <f>C7</f>
-        <v>"Neural Network" AND "Sustainable Developing"</v>
-      </c>
-      <c r="N40" s="17"/>
-      <c r="O40" s="17"/>
-      <c r="P40" s="17"/>
-      <c r="Q40" s="17"/>
-      <c r="R40" s="17"/>
-      <c r="S40" s="17"/>
+      <c r="M40" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>"Neural Network" AND "Sustainable Development"</v>
+      </c>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
     </row>
     <row r="41" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M41" s="17" t="str">
-        <f>C8</f>
+      <c r="M41" s="10" t="str">
+        <f t="shared" si="4"/>
         <v>"Neural Network" AND "Environment"</v>
       </c>
-      <c r="N41" s="17"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
-      <c r="Q41" s="17"/>
-      <c r="R41" s="17"/>
-      <c r="S41" s="17"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
     </row>
     <row r="42" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M42" s="17" t="str">
-        <f>C9</f>
-        <v>"Neural Network" AND "Environmental Sustaintability"</v>
-      </c>
-      <c r="N42" s="17"/>
-      <c r="O42" s="17"/>
-      <c r="P42" s="17"/>
-      <c r="Q42" s="17"/>
-      <c r="R42" s="17"/>
-      <c r="S42" s="17"/>
+      <c r="M42" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>"Neural Network" AND "Environmental Sustainability"</v>
+      </c>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="E12:K12"/>
     <mergeCell ref="E23:K23"/>
     <mergeCell ref="M33:S33"/>
+    <mergeCell ref="M12:S12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalizei Emerald Insight e Scopus, partindo para Springler
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Plácido\Documents\Faculdade\11 Semestre\Gestao de Qualidade\Artigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560CF1E7-2CB1-4993-B535-908FFD49DDE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A24908B-EDCC-4F98-A6F9-E8AD1AE3F846}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,9 +112,6 @@
     <t>Neural Network Environment</t>
   </si>
   <si>
-    <t>Neural Network Sustainable Developing</t>
-  </si>
-  <si>
     <t>Springer</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>Neural Network Environmental Sustainability</t>
   </si>
   <si>
-    <t>Review, Research and Case reports</t>
-  </si>
-  <si>
     <t>Número de Artigos Analisados</t>
   </si>
   <si>
@@ -158,6 +152,12 @@
   </si>
   <si>
     <t>"Neural Network" AND "Environmental Sustainability"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo </t>
+  </si>
+  <si>
+    <t>Neural Network Sustainable Development</t>
   </si>
 </sst>
 </file>
@@ -357,7 +357,223 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="49">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -929,105 +1145,130 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A6:F7" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A6:F7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A6:G7" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A6:G7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Artigo"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Autores"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ano de Publicação"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estratégia da Pesquisa"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Objetivo da Pesquisa"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Sustentabilidade"/>
+    <tableColumn id="6" xr3:uid="{064A3599-7589-40D8-A48A-75722D6B0988}" name="Tipo "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E9082B0C-C77E-4144-ABB3-2AFCBC27B540}" name="Table3" displayName="Table3" ref="E2:K11" totalsRowShown="0" headerRowDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E9082B0C-C77E-4144-ABB3-2AFCBC27B540}" name="Table3" displayName="Table3" ref="E2:K11" totalsRowShown="0" headerRowDxfId="48">
   <autoFilter ref="E2:K11" xr:uid="{B010B902-4089-4EDF-95EA-6510DE3263AD}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{150631A9-22E1-47B0-BF0B-E3226545937F}" name="Column1">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8DCACCD9-6A27-420A-A5EC-D230FB3DD3E1}" name="Science Direct" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{6641DD30-BFF3-4387-9774-4A7558C8F975}" name="Emerald Insight" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{DAD195B6-9347-4529-B450-D73CCDFBE75D}" name="Scopus" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{34F20F22-9351-4481-935A-8C2745791DD0}" name="Springler" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{BB081D5A-5346-4547-A641-31761151FB9D}" name="Wiley" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{4636F687-F30B-485D-8A92-E748AD5C8912}" name="Taylor &amp; Francis" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{8DCACCD9-6A27-420A-A5EC-D230FB3DD3E1}" name="Science Direct" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{6641DD30-BFF3-4387-9774-4A7558C8F975}" name="Emerald Insight" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{DAD195B6-9347-4529-B450-D73CCDFBE75D}" name="Scopus" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{34F20F22-9351-4481-935A-8C2745791DD0}" name="Springler" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{BB081D5A-5346-4547-A641-31761151FB9D}" name="Wiley" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{4636F687-F30B-485D-8A92-E748AD5C8912}" name="Taylor &amp; Francis" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6F8EB86C-85F1-4FBA-9FFC-B6D0058B3592}" name="Table35" displayName="Table35" ref="E13:K21" totalsRowShown="0" headerRowDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6F8EB86C-85F1-4FBA-9FFC-B6D0058B3592}" name="Table35" displayName="Table35" ref="E13:K22" totalsRowCount="1" headerRowDxfId="47">
   <autoFilter ref="E13:K21" xr:uid="{6D5004CA-553C-49B0-B5A0-226275053A1F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B76494C4-2327-4899-8567-C3C05E8F4CC7}" name="Column1">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D309A7D0-64F5-49E2-82A9-6BC2F06609A7}" name="Science Direct" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{8BB7FCBA-BACA-4910-9EF8-AB91065EFC17}" name="Emerald Insight" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{F918F495-5DA6-40C8-A18D-8D0ACDA320FD}" name="Scopus" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{5D0BBA33-8122-4273-9318-6B04EBDE10E2}" name="Springler" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{3B6A5EB3-0DE5-4170-9759-9BF25C23241A}" name="Wiley" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{170F1506-26AC-4697-8E2E-935DBA2D536D}" name="Taylor &amp; Francis" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{D309A7D0-64F5-49E2-82A9-6BC2F06609A7}" name="Science Direct" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="5">
+      <totalsRowFormula>SUM(Table35[Science Direct])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{8BB7FCBA-BACA-4910-9EF8-AB91065EFC17}" name="Emerald Insight" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="4">
+      <totalsRowFormula>SUM(Table35[Emerald Insight])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F918F495-5DA6-40C8-A18D-8D0ACDA320FD}" name="Scopus" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="3">
+      <totalsRowFormula>SUM(Table35[Scopus])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{5D0BBA33-8122-4273-9318-6B04EBDE10E2}" name="Springler" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="2">
+      <totalsRowFormula>SUM(Table35[Springler])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{3B6A5EB3-0DE5-4170-9759-9BF25C23241A}" name="Wiley" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="1">
+      <totalsRowFormula>SUM(Table35[Wiley])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{170F1506-26AC-4697-8E2E-935DBA2D536D}" name="Taylor &amp; Francis" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="0">
+      <totalsRowFormula>SUM(Table35[Taylor &amp; Francis])</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CD1481DA-7A29-4C6A-99A4-BB9A73AC5AAE}" name="Table356" displayName="Table356" ref="E24:K32" totalsRowShown="0" headerRowDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CD1481DA-7A29-4C6A-99A4-BB9A73AC5AAE}" name="Table356" displayName="Table356" ref="E24:K32" totalsRowShown="0" headerRowDxfId="46">
   <autoFilter ref="E24:K32" xr:uid="{325C82D0-9CFB-45D4-A270-FC6432082374}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{24654240-E379-4C9A-9DCD-65C789D335AB}" name="Column1">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{639EB9D1-B2B4-4E0F-8725-AFB812C9A65D}" name="Science Direct" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{BDA00B13-6195-44C0-99E4-22674588FB32}" name="Emerald Insight" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{CD7A3BC0-4322-4169-B82B-92D2BCD379A0}" name="Scopus" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{AEB54831-9168-44FC-A3FB-36C3901C1772}" name="Springler" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{9D108FDF-29DF-4855-825C-22556E2C6F9F}" name="Wiley" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{DC271623-6492-4738-A374-609DED940358}" name="Taylor &amp; Francis" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{639EB9D1-B2B4-4E0F-8725-AFB812C9A65D}" name="Science Direct" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{BDA00B13-6195-44C0-99E4-22674588FB32}" name="Emerald Insight" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{CD7A3BC0-4322-4169-B82B-92D2BCD379A0}" name="Scopus" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{AEB54831-9168-44FC-A3FB-36C3901C1772}" name="Springler" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{9D108FDF-29DF-4855-825C-22556E2C6F9F}" name="Wiley" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{DC271623-6492-4738-A374-609DED940358}" name="Taylor &amp; Francis" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AC928D1D-B98E-40EA-A207-C233D64396A2}" name="Table37" displayName="Table37" ref="M34:S42" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AC928D1D-B98E-40EA-A207-C233D64396A2}" name="Table37" displayName="Table37" ref="M34:S42" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="M34:S42" xr:uid="{67ACFE52-40D3-4D5B-9587-380B01CA9349}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CC58C69A-3BD4-439F-8E2A-78CFCFA772E9}" name="Column1" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{CC58C69A-3BD4-439F-8E2A-78CFCFA772E9}" name="Column1" dataDxfId="43">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{6752AC08-A118-44B2-9200-921CA1F8335B}" name="Science Direct" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{0472B21D-97B3-421D-B264-C2DE2E81F3BF}" name="Emerald Insight" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{EDB81E1A-540C-49BE-8621-D2F785CFDE5E}" name="Scopus" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{F477D8B8-98A5-4C44-83F3-C0FFBA22D4AD}" name="Springler" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{F947E302-3405-4752-8179-B2C47811F385}" name="Wiley" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{08B07A72-C239-4B61-91DE-CF31F091EA4B}" name="Taylor &amp; Francis" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{6752AC08-A118-44B2-9200-921CA1F8335B}" name="Science Direct" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{0472B21D-97B3-421D-B264-C2DE2E81F3BF}" name="Emerald Insight" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{EDB81E1A-540C-49BE-8621-D2F785CFDE5E}" name="Scopus" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{F477D8B8-98A5-4C44-83F3-C0FFBA22D4AD}" name="Springler" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{F947E302-3405-4752-8179-B2C47811F385}" name="Wiley" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{08B07A72-C239-4B61-91DE-CF31F091EA4B}" name="Taylor &amp; Francis" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{49435503-B1E7-4724-AFF1-275C704DC8E8}" name="Table33" displayName="Table33" ref="M13:S21" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{49435503-B1E7-4724-AFF1-275C704DC8E8}" name="Table33" displayName="Table33" ref="M13:S22" totalsRowCount="1" headerRowDxfId="36">
   <autoFilter ref="M13:S21" xr:uid="{1928454F-FA0E-4F92-AA13-866388A59E12}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D56F5F81-C1E6-46F7-ADE0-F94365FD3D3D}" name="Column1">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{611CC9E7-DBC7-4A7A-AED8-479F52685EA4}" name="Science Direct" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{EEDB19DA-96B1-4BE3-A9E8-30B7950DCCA0}" name="Emerald Insight" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{232281CB-02F4-4E71-8764-3B40A5B0AA63}" name="Scopus" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{3686983C-0E8E-47E0-974B-7884E8A32FE1}" name="Springler" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{B64EF221-003C-4B41-9901-A7FC32144AE1}" name="Wiley" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{CA984F23-3162-4D75-BE65-53769D2B4FF8}" name="Taylor &amp; Francis" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{611CC9E7-DBC7-4A7A-AED8-479F52685EA4}" name="Science Direct" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="11">
+      <totalsRowFormula>SUM(Table33[Science Direct])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{EEDB19DA-96B1-4BE3-A9E8-30B7950DCCA0}" name="Emerald Insight" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="10">
+      <totalsRowFormula>SUM(Table33[Emerald Insight])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{232281CB-02F4-4E71-8764-3B40A5B0AA63}" name="Scopus" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="9">
+      <totalsRowFormula>SUM(Table33[Scopus])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{3686983C-0E8E-47E0-974B-7884E8A32FE1}" name="Springler" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="8">
+      <totalsRowFormula>SUM(Table33[Springler])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{B64EF221-003C-4B41-9901-A7FC32144AE1}" name="Wiley" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="7">
+      <totalsRowFormula>SUM(Table33[Wiley])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{CA984F23-3162-4D75-BE65-53769D2B4FF8}" name="Taylor &amp; Francis" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="6">
+      <totalsRowFormula>SUM(Table33[Taylor &amp; Francis])</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1333,7 +1574,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,6 +1675,9 @@
       </c>
       <c r="F6" t="s">
         <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1456,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="J9" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,7 +1733,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
@@ -1504,10 +1748,10 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>16</v>
@@ -1533,7 +1777,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E3" t="str">
         <f>C2</f>
@@ -1546,9 +1790,11 @@
         <v>627</v>
       </c>
       <c r="H3" s="19">
-        <v>497</v>
-      </c>
-      <c r="I3" s="19"/>
+        <v>17926</v>
+      </c>
+      <c r="I3" s="19">
+        <v>4339</v>
+      </c>
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
     </row>
@@ -1561,7 +1807,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" ref="E4:E10" si="0">C3</f>
-        <v>Neural Network Sustainable Developing</v>
+        <v>Neural Network Sustainable Development</v>
       </c>
       <c r="F4" s="19">
         <v>44376</v>
@@ -1569,28 +1815,38 @@
       <c r="G4" s="19">
         <v>1052</v>
       </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="H4" s="19">
+        <v>1198</v>
+      </c>
+      <c r="I4" s="19">
+        <v>8190</v>
+      </c>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
     </row>
     <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
         <v>Neural Network Environment</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="19">
+        <v>130134</v>
+      </c>
       <c r="G5" s="19">
         <v>3278</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
+      <c r="H5" s="19">
+        <v>28659</v>
+      </c>
+      <c r="I5" s="19">
+        <v>129120</v>
+      </c>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
     </row>
@@ -1599,16 +1855,24 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
         <v>Neural Network Environmental Sustainability</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
+      <c r="F6" s="19">
+        <v>23038</v>
+      </c>
+      <c r="G6" s="19">
+        <v>567</v>
+      </c>
+      <c r="H6" s="19">
+        <v>156</v>
+      </c>
+      <c r="I6" s="19">
+        <v>3056</v>
+      </c>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
     </row>
@@ -1617,7 +1881,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -1629,14 +1893,16 @@
       <c r="G7" s="19">
         <v>123</v>
       </c>
-      <c r="H7" s="19"/>
+      <c r="H7" s="19">
+        <v>16366</v>
+      </c>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -1646,24 +1912,32 @@
         <v>2557</v>
       </c>
       <c r="G8" s="19">
-        <v>66</v>
-      </c>
-      <c r="H8" s="19"/>
+        <v>67</v>
+      </c>
+      <c r="H8" s="19">
+        <v>993</v>
+      </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
         <v>"Neural Network" AND "Environment"</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="F9" s="19">
+        <v>86616</v>
+      </c>
+      <c r="G9" s="19">
+        <v>1450</v>
+      </c>
+      <c r="H9" s="19">
+        <v>26875</v>
+      </c>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
@@ -1673,30 +1947,48 @@
         <f t="shared" si="0"/>
         <v>"Neural Network" AND "Environmental Sustainability"</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="F10" s="19">
+        <v>670</v>
+      </c>
+      <c r="G10" s="19">
+        <v>23</v>
+      </c>
+      <c r="H10" s="19">
+        <v>53</v>
+      </c>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="E11">
-        <f>C10</f>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F11" s="20">
+        <f>SUM(F3:F10)</f>
+        <v>360504</v>
+      </c>
+      <c r="G11" s="20">
+        <f t="shared" ref="G11:K11" si="1">SUM(G3:G10)</f>
+        <v>7187</v>
+      </c>
+      <c r="H11" s="20">
+        <f t="shared" si="1"/>
+        <v>92226</v>
+      </c>
+      <c r="I11" s="20">
+        <f t="shared" si="1"/>
+        <v>144705</v>
+      </c>
+      <c r="J11" s="20">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
+      <c r="K11" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="E12" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -1705,7 +1997,7 @@
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="M12" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
@@ -1716,7 +2008,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>16</v>
@@ -1737,7 +2029,7 @@
         <v>20</v>
       </c>
       <c r="M13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N13" s="9" t="s">
         <v>16</v>
@@ -1772,7 +2064,9 @@
       <c r="H14" s="19">
         <v>260</v>
       </c>
-      <c r="I14" s="19"/>
+      <c r="I14" s="19">
+        <v>1774</v>
+      </c>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
       <c r="M14" t="str">
@@ -1785,15 +2079,19 @@
       <c r="O14" s="19">
         <v>60</v>
       </c>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
+      <c r="P14" s="19">
+        <v>200</v>
+      </c>
+      <c r="Q14" s="19">
+        <v>60</v>
+      </c>
       <c r="R14" s="19"/>
       <c r="S14" s="19"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E15" t="str">
-        <f t="shared" ref="E15:E21" si="1">C3</f>
-        <v>Neural Network Sustainable Developing</v>
+        <f t="shared" ref="E15:E21" si="2">C3</f>
+        <v>Neural Network Sustainable Development</v>
       </c>
       <c r="F15" s="19">
         <v>22709</v>
@@ -1801,13 +2099,17 @@
       <c r="G15" s="19">
         <v>1052</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+      <c r="H15" s="19">
+        <v>382</v>
+      </c>
+      <c r="I15" s="19">
+        <v>3264</v>
+      </c>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
       <c r="M15" t="str">
-        <f t="shared" ref="M15:M21" si="2">C3</f>
-        <v>Neural Network Sustainable Developing</v>
+        <f t="shared" ref="M15:M21" si="3">C3</f>
+        <v>Neural Network Sustainable Development</v>
       </c>
       <c r="N15" s="19">
         <v>75</v>
@@ -1815,62 +2117,92 @@
       <c r="O15" s="19">
         <v>100</v>
       </c>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
+      <c r="P15" s="19">
+        <v>200</v>
+      </c>
+      <c r="Q15" s="19">
+        <v>80</v>
+      </c>
       <c r="R15" s="19"/>
       <c r="S15" s="19"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Neural Network Environment</v>
       </c>
-      <c r="F16" s="19"/>
+      <c r="F16" s="19">
+        <v>67706</v>
+      </c>
       <c r="G16" s="19">
         <v>3278</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="H16" s="19">
+        <v>8977</v>
+      </c>
+      <c r="I16" s="19">
+        <v>38355</v>
+      </c>
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
       <c r="M16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Neural Network Environment</v>
       </c>
-      <c r="N16" s="19"/>
+      <c r="N16" s="19">
+        <v>50</v>
+      </c>
       <c r="O16" s="19">
         <v>65</v>
       </c>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
+      <c r="P16" s="19">
+        <v>40</v>
+      </c>
+      <c r="Q16" s="19">
+        <v>40</v>
+      </c>
       <c r="R16" s="19"/>
       <c r="S16" s="19"/>
     </row>
     <row r="17" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Neural Network Environmental Sustainability</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="F17" s="19">
+        <v>12089</v>
+      </c>
+      <c r="G17" s="19">
+        <v>567</v>
+      </c>
+      <c r="H17" s="19">
+        <v>78</v>
+      </c>
+      <c r="I17" s="19">
+        <v>1329</v>
+      </c>
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
       <c r="M17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Neural Network Environmental Sustainability</v>
       </c>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
+      <c r="N17" s="19">
+        <v>200</v>
+      </c>
+      <c r="O17" s="19">
+        <v>40</v>
+      </c>
+      <c r="P17" s="19">
+        <v>78</v>
+      </c>
       <c r="Q17" s="19"/>
       <c r="R17" s="19"/>
       <c r="S17" s="19"/>
     </row>
     <row r="18" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>"Neural Network" AND "Sustainability"</v>
       </c>
       <c r="F18" s="18">
@@ -1879,12 +2211,14 @@
       <c r="G18" s="19">
         <v>123</v>
       </c>
-      <c r="H18" s="19"/>
+      <c r="H18" s="19">
+        <v>253</v>
+      </c>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
       <c r="M18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"Neural Network" AND "Sustainability"</v>
       </c>
       <c r="N18" s="18">
@@ -1893,84 +2227,168 @@
       <c r="O18" s="19">
         <v>50</v>
       </c>
-      <c r="P18" s="19"/>
+      <c r="P18" s="19">
+        <v>100</v>
+      </c>
       <c r="Q18" s="19"/>
       <c r="R18" s="19"/>
       <c r="S18" s="19"/>
     </row>
     <row r="19" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>"Neural Network" AND "Sustainable Development"</v>
       </c>
       <c r="F19" s="19">
         <v>1741</v>
       </c>
       <c r="G19" s="19">
-        <v>66</v>
-      </c>
-      <c r="H19" s="19"/>
+        <v>67</v>
+      </c>
+      <c r="H19" s="19">
+        <v>304</v>
+      </c>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
       <c r="M19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"Neural Network" AND "Sustainable Development"</v>
       </c>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
+      <c r="N19" s="19">
+        <v>100</v>
+      </c>
+      <c r="O19" s="19">
+        <v>40</v>
+      </c>
+      <c r="P19" s="19">
+        <v>100</v>
+      </c>
       <c r="Q19" s="19"/>
       <c r="R19" s="19"/>
       <c r="S19" s="19"/>
     </row>
     <row r="20" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>"Neural Network" AND "Environment"</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="F20" s="19">
+        <v>48334</v>
+      </c>
+      <c r="G20" s="19">
+        <v>1450</v>
+      </c>
+      <c r="H20" s="19">
+        <v>7850</v>
+      </c>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
       <c r="M20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"Neural Network" AND "Environment"</v>
       </c>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
+      <c r="N20" s="19">
+        <v>50</v>
+      </c>
+      <c r="O20" s="19">
+        <v>30</v>
+      </c>
+      <c r="P20" s="19">
+        <v>40</v>
+      </c>
       <c r="Q20" s="19"/>
       <c r="R20" s="19"/>
       <c r="S20" s="19"/>
     </row>
     <row r="21" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>"Neural Network" AND "Environmental Sustainability"</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="F21" s="19">
+        <v>477</v>
+      </c>
+      <c r="G21" s="19">
+        <v>23</v>
+      </c>
+      <c r="H21" s="19">
+        <v>19</v>
+      </c>
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
       <c r="M21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>"Neural Network" AND "Environmental Sustainability"</v>
       </c>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
+      <c r="N21" s="19">
+        <v>60</v>
+      </c>
+      <c r="O21" s="19">
+        <v>23</v>
+      </c>
+      <c r="P21" s="19">
+        <v>19</v>
+      </c>
       <c r="Q21" s="19"/>
       <c r="R21" s="19"/>
       <c r="S21" s="19"/>
     </row>
+    <row r="22" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="F22" s="19">
+        <f>SUM(Table35[Science Direct])</f>
+        <v>196674</v>
+      </c>
+      <c r="G22" s="19">
+        <f>SUM(Table35[Emerald Insight])</f>
+        <v>7187</v>
+      </c>
+      <c r="H22" s="19">
+        <f>SUM(Table35[Scopus])</f>
+        <v>18123</v>
+      </c>
+      <c r="I22" s="19">
+        <f>SUM(Table35[Springler])</f>
+        <v>44722</v>
+      </c>
+      <c r="J22" s="19">
+        <f>SUM(Table35[Wiley])</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="19">
+        <f>SUM(Table35[Taylor &amp; Francis])</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="19">
+        <f>SUM(Table33[Science Direct])</f>
+        <v>810</v>
+      </c>
+      <c r="O22" s="19">
+        <f>SUM(Table33[Emerald Insight])</f>
+        <v>408</v>
+      </c>
+      <c r="P22" s="19">
+        <f>SUM(Table33[Scopus])</f>
+        <v>777</v>
+      </c>
+      <c r="Q22" s="19">
+        <f>SUM(Table33[Springler])</f>
+        <v>180</v>
+      </c>
+      <c r="R22" s="19">
+        <f>SUM(Table33[Wiley])</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="19">
+        <f>SUM(Table33[Taylor &amp; Francis])</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="23" spans="5:19" ht="21" x14ac:dyDescent="0.35">
       <c r="E23" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
@@ -1981,7 +2399,7 @@
     </row>
     <row r="24" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>16</v>
@@ -2016,8 +2434,8 @@
     </row>
     <row r="26" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E26" t="str">
-        <f t="shared" ref="E26:E32" si="3">C3</f>
-        <v>Neural Network Sustainable Developing</v>
+        <f t="shared" ref="E26:E32" si="4">C3</f>
+        <v>Neural Network Sustainable Development</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -2028,7 +2446,7 @@
     </row>
     <row r="27" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Neural Network Environment</v>
       </c>
       <c r="F27" s="19"/>
@@ -2040,7 +2458,7 @@
     </row>
     <row r="28" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Neural Network Environmental Sustainability</v>
       </c>
       <c r="F28" s="19"/>
@@ -2052,7 +2470,7 @@
     </row>
     <row r="29" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>"Neural Network" AND "Sustainability"</v>
       </c>
       <c r="F29" s="18"/>
@@ -2064,7 +2482,7 @@
     </row>
     <row r="30" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>"Neural Network" AND "Sustainable Development"</v>
       </c>
       <c r="F30" s="19"/>
@@ -2076,7 +2494,7 @@
     </row>
     <row r="31" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>"Neural Network" AND "Environment"</v>
       </c>
       <c r="F31" s="19"/>
@@ -2088,7 +2506,7 @@
     </row>
     <row r="32" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>"Neural Network" AND "Environmental Sustainability"</v>
       </c>
       <c r="F32" s="19"/>
@@ -2100,7 +2518,7 @@
     </row>
     <row r="33" spans="13:19" ht="21" x14ac:dyDescent="0.35">
       <c r="M33" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N33" s="16"/>
       <c r="O33" s="16"/>
@@ -2111,7 +2529,7 @@
     </row>
     <row r="34" spans="13:19" x14ac:dyDescent="0.25">
       <c r="M34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N34" s="9" t="s">
         <v>16</v>
@@ -2134,11 +2552,11 @@
     </row>
     <row r="35" spans="13:19" ht="30" x14ac:dyDescent="0.25">
       <c r="M35" s="10" t="str">
-        <f t="shared" ref="M35:M42" si="4">C2</f>
+        <f t="shared" ref="M35:M42" si="5">C2</f>
         <v>Neural Network Sustainability</v>
       </c>
       <c r="N35" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
@@ -2148,8 +2566,8 @@
     </row>
     <row r="36" spans="13:19" x14ac:dyDescent="0.25">
       <c r="M36" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>Neural Network Sustainable Developing</v>
+        <f t="shared" si="5"/>
+        <v>Neural Network Sustainable Development</v>
       </c>
       <c r="N36" s="10"/>
       <c r="O36" s="10"/>
@@ -2160,7 +2578,7 @@
     </row>
     <row r="37" spans="13:19" x14ac:dyDescent="0.25">
       <c r="M37" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Neural Network Environment</v>
       </c>
       <c r="N37" s="10"/>
@@ -2172,7 +2590,7 @@
     </row>
     <row r="38" spans="13:19" x14ac:dyDescent="0.25">
       <c r="M38" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Neural Network Environmental Sustainability</v>
       </c>
       <c r="N38" s="10"/>
@@ -2184,7 +2602,7 @@
     </row>
     <row r="39" spans="13:19" x14ac:dyDescent="0.25">
       <c r="M39" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>"Neural Network" AND "Sustainability"</v>
       </c>
       <c r="N39" s="10"/>
@@ -2196,7 +2614,7 @@
     </row>
     <row r="40" spans="13:19" x14ac:dyDescent="0.25">
       <c r="M40" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>"Neural Network" AND "Sustainable Development"</v>
       </c>
       <c r="N40" s="10"/>
@@ -2208,7 +2626,7 @@
     </row>
     <row r="41" spans="13:19" x14ac:dyDescent="0.25">
       <c r="M41" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>"Neural Network" AND "Environment"</v>
       </c>
       <c r="N41" s="10"/>
@@ -2220,7 +2638,7 @@
     </row>
     <row r="42" spans="13:19" x14ac:dyDescent="0.25">
       <c r="M42" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>"Neural Network" AND "Environmental Sustainability"</v>
       </c>
       <c r="N42" s="10"/>

</xml_diff>

<commit_message>
Falta pouco para finalizar Taylor & Francis e começar a escrever o artigo
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Plácido\Documents\Faculdade\11 Semestre\Gestao de Qualidade\Artigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A24908B-EDCC-4F98-A6F9-E8AD1AE3F846}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD54DBB-83F7-4EEB-8FDD-3E98C18A92EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1185,22 +1185,22 @@
     <tableColumn id="1" xr3:uid="{B76494C4-2327-4899-8567-C3C05E8F4CC7}" name="Column1">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D309A7D0-64F5-49E2-82A9-6BC2F06609A7}" name="Science Direct" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="5">
+    <tableColumn id="2" xr3:uid="{D309A7D0-64F5-49E2-82A9-6BC2F06609A7}" name="Science Direct" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="11">
       <totalsRowFormula>SUM(Table35[Science Direct])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8BB7FCBA-BACA-4910-9EF8-AB91065EFC17}" name="Emerald Insight" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="4">
+    <tableColumn id="3" xr3:uid="{8BB7FCBA-BACA-4910-9EF8-AB91065EFC17}" name="Emerald Insight" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="10">
       <totalsRowFormula>SUM(Table35[Emerald Insight])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F918F495-5DA6-40C8-A18D-8D0ACDA320FD}" name="Scopus" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="3">
+    <tableColumn id="4" xr3:uid="{F918F495-5DA6-40C8-A18D-8D0ACDA320FD}" name="Scopus" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="9">
       <totalsRowFormula>SUM(Table35[Scopus])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5D0BBA33-8122-4273-9318-6B04EBDE10E2}" name="Springler" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="2">
+    <tableColumn id="5" xr3:uid="{5D0BBA33-8122-4273-9318-6B04EBDE10E2}" name="Springler" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="8">
       <totalsRowFormula>SUM(Table35[Springler])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3B6A5EB3-0DE5-4170-9759-9BF25C23241A}" name="Wiley" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="1">
+    <tableColumn id="6" xr3:uid="{3B6A5EB3-0DE5-4170-9759-9BF25C23241A}" name="Wiley" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="7">
       <totalsRowFormula>SUM(Table35[Wiley])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{170F1506-26AC-4697-8E2E-935DBA2D536D}" name="Taylor &amp; Francis" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="0">
+    <tableColumn id="7" xr3:uid="{170F1506-26AC-4697-8E2E-935DBA2D536D}" name="Taylor &amp; Francis" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="6">
       <totalsRowFormula>SUM(Table35[Taylor &amp; Francis])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1215,12 +1215,12 @@
     <tableColumn id="1" xr3:uid="{24654240-E379-4C9A-9DCD-65C789D335AB}" name="Column1">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{639EB9D1-B2B4-4E0F-8725-AFB812C9A65D}" name="Science Direct" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{BDA00B13-6195-44C0-99E4-22674588FB32}" name="Emerald Insight" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{CD7A3BC0-4322-4169-B82B-92D2BCD379A0}" name="Scopus" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{AEB54831-9168-44FC-A3FB-36C3901C1772}" name="Springler" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{9D108FDF-29DF-4855-825C-22556E2C6F9F}" name="Wiley" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{DC271623-6492-4738-A374-609DED940358}" name="Taylor &amp; Francis" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{639EB9D1-B2B4-4E0F-8725-AFB812C9A65D}" name="Science Direct" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{BDA00B13-6195-44C0-99E4-22674588FB32}" name="Emerald Insight" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{CD7A3BC0-4322-4169-B82B-92D2BCD379A0}" name="Scopus" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{AEB54831-9168-44FC-A3FB-36C3901C1772}" name="Springler" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{9D108FDF-29DF-4855-825C-22556E2C6F9F}" name="Wiley" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{DC271623-6492-4738-A374-609DED940358}" name="Taylor &amp; Francis" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1251,22 +1251,22 @@
     <tableColumn id="1" xr3:uid="{D56F5F81-C1E6-46F7-ADE0-F94365FD3D3D}" name="Column1">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{611CC9E7-DBC7-4A7A-AED8-479F52685EA4}" name="Science Direct" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="11">
+    <tableColumn id="2" xr3:uid="{611CC9E7-DBC7-4A7A-AED8-479F52685EA4}" name="Science Direct" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="5">
       <totalsRowFormula>SUM(Table33[Science Direct])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EEDB19DA-96B1-4BE3-A9E8-30B7950DCCA0}" name="Emerald Insight" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="10">
+    <tableColumn id="3" xr3:uid="{EEDB19DA-96B1-4BE3-A9E8-30B7950DCCA0}" name="Emerald Insight" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="4">
       <totalsRowFormula>SUM(Table33[Emerald Insight])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{232281CB-02F4-4E71-8764-3B40A5B0AA63}" name="Scopus" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="9">
+    <tableColumn id="4" xr3:uid="{232281CB-02F4-4E71-8764-3B40A5B0AA63}" name="Scopus" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="3">
       <totalsRowFormula>SUM(Table33[Scopus])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3686983C-0E8E-47E0-974B-7884E8A32FE1}" name="Springler" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="8">
+    <tableColumn id="5" xr3:uid="{3686983C-0E8E-47E0-974B-7884E8A32FE1}" name="Springler" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="2">
       <totalsRowFormula>SUM(Table33[Springler])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B64EF221-003C-4B41-9901-A7FC32144AE1}" name="Wiley" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="7">
+    <tableColumn id="6" xr3:uid="{B64EF221-003C-4B41-9901-A7FC32144AE1}" name="Wiley" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="1">
       <totalsRowFormula>SUM(Table33[Wiley])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{CA984F23-3162-4D75-BE65-53769D2B4FF8}" name="Taylor &amp; Francis" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="6">
+    <tableColumn id="7" xr3:uid="{CA984F23-3162-4D75-BE65-53769D2B4FF8}" name="Taylor &amp; Francis" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="0">
       <totalsRowFormula>SUM(Table33[Taylor &amp; Francis])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1700,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J9" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="L4" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,8 +1795,12 @@
       <c r="I3" s="19">
         <v>4339</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
+      <c r="J3" s="19">
+        <v>5440</v>
+      </c>
+      <c r="K3" s="19">
+        <v>4610</v>
+      </c>
     </row>
     <row r="4" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1821,8 +1825,12 @@
       <c r="I4" s="19">
         <v>8190</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
+      <c r="J4" s="19">
+        <v>27414</v>
+      </c>
+      <c r="K4" s="19">
+        <v>11745</v>
+      </c>
     </row>
     <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -1847,8 +1855,12 @@
       <c r="I5" s="19">
         <v>129120</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
+      <c r="J5" s="19">
+        <v>69147</v>
+      </c>
+      <c r="K5" s="19">
+        <v>32024</v>
+      </c>
     </row>
     <row r="6" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -1873,8 +1885,12 @@
       <c r="I6" s="19">
         <v>3056</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
+      <c r="J6" s="19">
+        <v>4961</v>
+      </c>
+      <c r="K6" s="19">
+        <v>4306</v>
+      </c>
     </row>
     <row r="7" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -1896,9 +1912,15 @@
       <c r="H7" s="19">
         <v>16366</v>
       </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
+      <c r="I7" s="19">
+        <v>3453</v>
+      </c>
+      <c r="J7" s="19">
+        <v>773</v>
+      </c>
+      <c r="K7" s="19">
+        <v>1559</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -1917,8 +1939,12 @@
       <c r="H8" s="19">
         <v>993</v>
       </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
+      <c r="I8" s="19">
+        <v>2506</v>
+      </c>
+      <c r="J8" s="19">
+        <v>238</v>
+      </c>
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1938,8 +1964,12 @@
       <c r="H9" s="19">
         <v>26875</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
+      <c r="I9" s="19">
+        <v>94925</v>
+      </c>
+      <c r="J9" s="19">
+        <v>13442</v>
+      </c>
       <c r="K9" s="19"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1956,8 +1986,12 @@
       <c r="H10" s="19">
         <v>53</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
+      <c r="I10" s="19">
+        <v>308</v>
+      </c>
+      <c r="J10" s="19">
+        <v>59</v>
+      </c>
       <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1975,15 +2009,15 @@
       </c>
       <c r="I11" s="20">
         <f t="shared" si="1"/>
-        <v>144705</v>
+        <v>245897</v>
       </c>
       <c r="J11" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>121474</v>
       </c>
       <c r="K11" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>54244</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="21" x14ac:dyDescent="0.35">
@@ -2067,8 +2101,12 @@
       <c r="I14" s="19">
         <v>1774</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
+      <c r="J14" s="19">
+        <v>2950</v>
+      </c>
+      <c r="K14" s="19">
+        <v>3289</v>
+      </c>
       <c r="M14" t="str">
         <f>C2</f>
         <v>Neural Network Sustainability</v>
@@ -2085,8 +2123,12 @@
       <c r="Q14" s="19">
         <v>60</v>
       </c>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
+      <c r="R14" s="19">
+        <v>40</v>
+      </c>
+      <c r="S14" s="19">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E15" t="str">
@@ -2105,8 +2147,12 @@
       <c r="I15" s="19">
         <v>3264</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
+      <c r="J15" s="19">
+        <v>12553</v>
+      </c>
+      <c r="K15" s="19">
+        <v>7383</v>
+      </c>
       <c r="M15" t="str">
         <f t="shared" ref="M15:M21" si="3">C3</f>
         <v>Neural Network Sustainable Development</v>
@@ -2123,8 +2169,12 @@
       <c r="Q15" s="19">
         <v>80</v>
       </c>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
+      <c r="R15" s="19">
+        <v>60</v>
+      </c>
+      <c r="S15" s="19">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E16" t="str">
@@ -2143,8 +2193,12 @@
       <c r="I16" s="19">
         <v>38355</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
+      <c r="J16" s="19">
+        <v>31700</v>
+      </c>
+      <c r="K16" s="19">
+        <v>19240</v>
+      </c>
       <c r="M16" t="str">
         <f t="shared" si="3"/>
         <v>Neural Network Environment</v>
@@ -2161,8 +2215,12 @@
       <c r="Q16" s="19">
         <v>40</v>
       </c>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
+      <c r="R16" s="19">
+        <v>20</v>
+      </c>
+      <c r="S16" s="19">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E17" t="str">
@@ -2181,8 +2239,12 @@
       <c r="I17" s="19">
         <v>1329</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
+      <c r="J17" s="19">
+        <v>2674</v>
+      </c>
+      <c r="K17" s="19">
+        <v>3055</v>
+      </c>
       <c r="M17" t="str">
         <f t="shared" si="3"/>
         <v>Neural Network Environmental Sustainability</v>
@@ -2196,9 +2258,15 @@
       <c r="P17" s="19">
         <v>78</v>
       </c>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
+      <c r="Q17" s="19">
+        <v>80</v>
+      </c>
+      <c r="R17" s="19">
+        <v>60</v>
+      </c>
+      <c r="S17" s="19">
+        <v>60</v>
+      </c>
     </row>
     <row r="18" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E18" t="str">
@@ -2214,9 +2282,15 @@
       <c r="H18" s="19">
         <v>253</v>
       </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
+      <c r="I18" s="19">
+        <v>1459</v>
+      </c>
+      <c r="J18" s="19">
+        <v>411</v>
+      </c>
+      <c r="K18" s="19">
+        <v>1145</v>
+      </c>
       <c r="M18" t="str">
         <f t="shared" si="3"/>
         <v>"Neural Network" AND "Sustainability"</v>
@@ -2230,9 +2304,15 @@
       <c r="P18" s="19">
         <v>100</v>
       </c>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
+      <c r="Q18" s="19">
+        <v>100</v>
+      </c>
+      <c r="R18" s="19">
+        <v>20</v>
+      </c>
+      <c r="S18" s="19">
+        <v>70</v>
+      </c>
     </row>
     <row r="19" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E19" t="str">
@@ -2248,11 +2328,15 @@
       <c r="H19" s="19">
         <v>304</v>
       </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
+      <c r="I19" s="19">
+        <v>1041</v>
+      </c>
+      <c r="J19" s="19">
+        <v>114</v>
+      </c>
       <c r="K19" s="19"/>
       <c r="M19" t="str">
-        <f t="shared" si="3"/>
+        <f>C7</f>
         <v>"Neural Network" AND "Sustainable Development"</v>
       </c>
       <c r="N19" s="19">
@@ -2264,8 +2348,12 @@
       <c r="P19" s="19">
         <v>100</v>
       </c>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
+      <c r="Q19" s="19">
+        <v>80</v>
+      </c>
+      <c r="R19" s="19">
+        <v>20</v>
+      </c>
       <c r="S19" s="19"/>
     </row>
     <row r="20" spans="5:19" x14ac:dyDescent="0.25">
@@ -2282,8 +2370,12 @@
       <c r="H20" s="19">
         <v>7850</v>
       </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
+      <c r="I20" s="19">
+        <v>28492</v>
+      </c>
+      <c r="J20" s="19">
+        <v>5747</v>
+      </c>
       <c r="K20" s="19"/>
       <c r="M20" t="str">
         <f t="shared" si="3"/>
@@ -2298,8 +2390,12 @@
       <c r="P20" s="19">
         <v>40</v>
       </c>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
+      <c r="Q20" s="19">
+        <v>20</v>
+      </c>
+      <c r="R20" s="19">
+        <v>60</v>
+      </c>
       <c r="S20" s="19"/>
     </row>
     <row r="21" spans="5:19" x14ac:dyDescent="0.25">
@@ -2316,8 +2412,12 @@
       <c r="H21" s="19">
         <v>19</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
+      <c r="I21" s="19">
+        <v>154</v>
+      </c>
+      <c r="J21" s="19">
+        <v>40</v>
+      </c>
       <c r="K21" s="19"/>
       <c r="M21" t="str">
         <f t="shared" si="3"/>
@@ -2332,8 +2432,12 @@
       <c r="P21" s="19">
         <v>19</v>
       </c>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
+      <c r="Q21" s="19">
+        <v>40</v>
+      </c>
+      <c r="R21" s="19">
+        <v>40</v>
+      </c>
       <c r="S21" s="19"/>
     </row>
     <row r="22" spans="5:19" x14ac:dyDescent="0.25">
@@ -2351,15 +2455,15 @@
       </c>
       <c r="I22" s="19">
         <f>SUM(Table35[Springler])</f>
-        <v>44722</v>
+        <v>75868</v>
       </c>
       <c r="J22" s="19">
         <f>SUM(Table35[Wiley])</f>
-        <v>0</v>
+        <v>56189</v>
       </c>
       <c r="K22" s="19">
         <f>SUM(Table35[Taylor &amp; Francis])</f>
-        <v>0</v>
+        <v>34112</v>
       </c>
       <c r="N22" s="19">
         <f>SUM(Table33[Science Direct])</f>
@@ -2375,15 +2479,15 @@
       </c>
       <c r="Q22" s="19">
         <f>SUM(Table33[Springler])</f>
-        <v>180</v>
+        <v>500</v>
       </c>
       <c r="R22" s="19">
         <f>SUM(Table33[Wiley])</f>
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="S22" s="19">
         <f>SUM(Table33[Taylor &amp; Francis])</f>
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="5:19" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Finalizei a busca por artigos, agora irei remover duplicatas e começar a extrair dados interessantes
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Plácido\Documents\Faculdade\11 Semestre\Gestao de Qualidade\Artigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD54DBB-83F7-4EEB-8FDD-3E98C18A92EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857680F1-B824-4354-A83C-A9553F3503A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>Uso de Redes Neurais no Contexto da Sustentabilidade</t>
   </si>
@@ -152,9 +152,6 @@
   </si>
   <si>
     <t>"Neural Network" AND "Environmental Sustainability"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo </t>
   </si>
   <si>
     <t>Neural Network Sustainable Development</t>
@@ -1145,16 +1142,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A6:G7" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A6:G7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A6:F7" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A6:F7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Artigo"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Autores"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ano de Publicação"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estratégia da Pesquisa"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Objetivo da Pesquisa"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Sustentabilidade"/>
-    <tableColumn id="6" xr3:uid="{064A3599-7589-40D8-A48A-75722D6B0988}" name="Tipo "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1571,10 +1567,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,11 +1582,11 @@
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1600,17 +1597,16 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="11" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="12"/>
-    </row>
-    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1621,43 +1617,42 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="6" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J3" s="14" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="6" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J4" s="14" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="6" t="s">
+      <c r="J4" s="14"/>
+      <c r="K4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1676,17 +1671,14 @@
       <c r="F6" t="s">
         <v>6</v>
       </c>
-      <c r="G6" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1698,10 +1690,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L4" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,7 +1770,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" t="str">
         <f>C2</f>
@@ -1945,7 +1938,9 @@
       <c r="J8" s="19">
         <v>238</v>
       </c>
-      <c r="K8" s="19"/>
+      <c r="K8" s="19">
+        <v>362</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
@@ -1970,7 +1965,9 @@
       <c r="J9" s="19">
         <v>13442</v>
       </c>
-      <c r="K9" s="19"/>
+      <c r="K9" s="19">
+        <v>10608</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E10" t="str">
@@ -1992,7 +1989,9 @@
       <c r="J10" s="19">
         <v>59</v>
       </c>
-      <c r="K10" s="19"/>
+      <c r="K10" s="19">
+        <v>54</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F11" s="20">
@@ -2017,7 +2016,7 @@
       </c>
       <c r="K11" s="20">
         <f t="shared" si="1"/>
-        <v>54244</v>
+        <v>65268</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="21" x14ac:dyDescent="0.35">
@@ -2334,7 +2333,9 @@
       <c r="J19" s="19">
         <v>114</v>
       </c>
-      <c r="K19" s="19"/>
+      <c r="K19" s="19">
+        <v>270</v>
+      </c>
       <c r="M19" t="str">
         <f>C7</f>
         <v>"Neural Network" AND "Sustainable Development"</v>
@@ -2354,7 +2355,9 @@
       <c r="R19" s="19">
         <v>20</v>
       </c>
-      <c r="S19" s="19"/>
+      <c r="S19" s="19">
+        <v>70</v>
+      </c>
     </row>
     <row r="20" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E20" t="str">
@@ -2376,7 +2379,9 @@
       <c r="J20" s="19">
         <v>5747</v>
       </c>
-      <c r="K20" s="19"/>
+      <c r="K20" s="19">
+        <v>6488</v>
+      </c>
       <c r="M20" t="str">
         <f t="shared" si="3"/>
         <v>"Neural Network" AND "Environment"</v>
@@ -2396,7 +2401,9 @@
       <c r="R20" s="19">
         <v>60</v>
       </c>
-      <c r="S20" s="19"/>
+      <c r="S20" s="19">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E21" t="str">
@@ -2418,7 +2425,9 @@
       <c r="J21" s="19">
         <v>40</v>
       </c>
-      <c r="K21" s="19"/>
+      <c r="K21" s="19">
+        <v>43</v>
+      </c>
       <c r="M21" t="str">
         <f t="shared" si="3"/>
         <v>"Neural Network" AND "Environmental Sustainability"</v>
@@ -2438,7 +2447,9 @@
       <c r="R21" s="19">
         <v>40</v>
       </c>
-      <c r="S21" s="19"/>
+      <c r="S21" s="19">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="5:19" x14ac:dyDescent="0.25">
       <c r="F22" s="19">
@@ -2463,7 +2474,7 @@
       </c>
       <c r="K22" s="19">
         <f>SUM(Table35[Taylor &amp; Francis])</f>
-        <v>34112</v>
+        <v>40913</v>
       </c>
       <c r="N22" s="19">
         <f>SUM(Table33[Science Direct])</f>
@@ -2487,7 +2498,7 @@
       </c>
       <c r="S22" s="19">
         <f>SUM(Table33[Taylor &amp; Francis])</f>
-        <v>270</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" spans="5:19" ht="21" x14ac:dyDescent="0.35">

</xml_diff>